<commit_message>
⚡️ evaluation end to end
</commit_message>
<xml_diff>
--- a/Berechnungen.xlsx
+++ b/Berechnungen.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/lenert/Thesis/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{387D046B-CCCC-1E49-82A6-371A5AFA6DBB}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{EA3AEF37-BA21-E745-97EF-AE55F4791D73}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="320" yWindow="500" windowWidth="24940" windowHeight="14400" xr2:uid="{FC04C70B-1B40-1547-8254-13E87224A8AC}"/>
   </bookViews>
@@ -36,7 +36,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="21" uniqueCount="10">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="23" uniqueCount="12">
   <si>
     <t>LeoLama</t>
   </si>
@@ -66,6 +66,12 @@
   </si>
   <si>
     <t>avg abweichung</t>
+  </si>
+  <si>
+    <t>Gold Answers</t>
+  </si>
+  <si>
+    <t>Extractive</t>
   </si>
 </sst>
 </file>
@@ -421,10 +427,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{2738F8A8-E061-E64D-BF94-F3AC06BA34D0}">
-  <dimension ref="A1:K28"/>
+  <dimension ref="A1:K35"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="K6" sqref="K6"/>
+    <sheetView tabSelected="1" topLeftCell="A15" workbookViewId="0">
+      <selection activeCell="D38" sqref="D38"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -723,6 +729,62 @@
     <row r="28" spans="1:11" x14ac:dyDescent="0.2">
       <c r="D28" s="1"/>
     </row>
+    <row r="31" spans="1:11" x14ac:dyDescent="0.2">
+      <c r="A31" t="s">
+        <v>10</v>
+      </c>
+      <c r="B31">
+        <v>10</v>
+      </c>
+      <c r="E31" t="s">
+        <v>11</v>
+      </c>
+      <c r="F31">
+        <v>34.5</v>
+      </c>
+    </row>
+    <row r="32" spans="1:11" x14ac:dyDescent="0.2">
+      <c r="B32">
+        <v>10.5</v>
+      </c>
+      <c r="F32">
+        <v>39</v>
+      </c>
+    </row>
+    <row r="33" spans="2:7" x14ac:dyDescent="0.2">
+      <c r="B33">
+        <v>10</v>
+      </c>
+      <c r="F33">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="34" spans="2:7" x14ac:dyDescent="0.2">
+      <c r="B34">
+        <v>14</v>
+      </c>
+      <c r="F34">
+        <v>16</v>
+      </c>
+    </row>
+    <row r="35" spans="2:7" x14ac:dyDescent="0.2">
+      <c r="B35">
+        <f>SUM(B31:B34)</f>
+        <v>44.5</v>
+      </c>
+      <c r="C35">
+        <f>B35/200</f>
+        <v>0.2225</v>
+      </c>
+      <c r="F35">
+        <f>SUM(F31:F34)</f>
+        <v>102.5</v>
+      </c>
+      <c r="G35">
+        <f>F35/200</f>
+        <v>0.51249999999999996</v>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.78740157499999996" bottom="0.78740157499999996" header="0.3" footer="0.3"/>
 </worksheet>

</xml_diff>